<commit_message>
fix comparison modes, use combine_excel_files(), fix column letters selection, change debug colors
</commit_message>
<xml_diff>
--- a/fileB.xlsx
+++ b/fileB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\az_dev\UPWORK\combine-xls.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFD6C0D-573B-444E-9508-FE72FD2AA325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0939317-AB5C-48DB-82EA-2FEE32DF75E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D486BA36-64EB-473E-8DB1-09E25233AE67}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>5yz7fafspka5h0acz4hus5yz7rti6yb9</t>
   </si>
   <si>
-    <t>Cal</t>
-  </si>
-  <si>
-    <t>Arnold</t>
-  </si>
-  <si>
     <t>256-242-9976</t>
   </si>
   <si>
@@ -108,12 +102,6 @@
     <t>walkin</t>
   </si>
   <si>
-    <t>Mc'Elroy</t>
-  </si>
-  <si>
-    <t>Stu</t>
-  </si>
-  <si>
     <t>(382)-719-2456</t>
   </si>
   <si>
@@ -129,12 +117,6 @@
     <t>mjr7u5nz6qic0e64vmjr7u5ycdf6akj6</t>
   </si>
   <si>
-    <t>Uncle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rico </t>
-  </si>
-  <si>
     <t>Oakville</t>
   </si>
   <si>
@@ -150,12 +132,6 @@
     <t>1gwg7</t>
   </si>
   <si>
-    <t>Renée</t>
-  </si>
-  <si>
-    <t>Liêvre</t>
-  </si>
-  <si>
     <t>956-717-9023</t>
   </si>
   <si>
@@ -172,6 +148,30 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>arnold</t>
+  </si>
+  <si>
+    <t>stu</t>
+  </si>
+  <si>
+    <t>mc'elroy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rico </t>
+  </si>
+  <si>
+    <t>renée</t>
+  </si>
+  <si>
+    <t>liêvre</t>
+  </si>
+  <si>
+    <t>ncle</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -579,16 +579,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -611,121 +611,121 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>9993457586</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>15</v>
@@ -734,16 +734,16 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>